<commit_message>
correccion del archivo Excel
</commit_message>
<xml_diff>
--- a/Ejemplo_100Reg..xlsx
+++ b/Ejemplo_100Reg..xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor\Source\Repos\SaxSolution\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="16515" windowHeight="6975" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="16515" windowHeight="6975"/>
   </bookViews>
   <sheets>
-    <sheet name="Celdas-Campo" sheetId="2" r:id="rId1"/>
-    <sheet name="Ejemplo" sheetId="1" r:id="rId2"/>
+    <sheet name="Ejemplo" sheetId="1" r:id="rId1"/>
+    <sheet name="Celdas-Campo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="450">
   <si>
     <t>Campo 1</t>
   </si>
@@ -1344,6 +1349,27 @@
   </si>
   <si>
     <t>FIDEICOMISO I.A. VIVA COLOMBIA 6063 - INGRESO POR</t>
+  </si>
+  <si>
+    <t>44179</t>
+  </si>
+  <si>
+    <t>5380</t>
+  </si>
+  <si>
+    <t>1150</t>
+  </si>
+  <si>
+    <t>2123</t>
+  </si>
+  <si>
+    <t>2036</t>
+  </si>
+  <si>
+    <t>5002</t>
+  </si>
+  <si>
+    <t>1044</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1378,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1874,7 +1900,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
@@ -1937,6 +1963,7 @@
     <cellStyle name="Cálculo" xfId="12" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="14" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="3" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="6" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="19" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="23" builtinId="33" customBuiltin="1"/>
@@ -1958,7 +1985,6 @@
     <cellStyle name="Texto de advertencia" xfId="15" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="17" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="3" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
@@ -1968,6 +1994,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2016,7 +2045,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2051,7 +2080,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2260,1074 +2289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F62"/>
-  <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D4" s="1">
-        <v>30</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="D7" s="1">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="D8" s="1">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="D9" s="1">
-        <v>700</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="D10" s="1">
-        <v>700</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="D11" s="1">
-        <v>7</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>50</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>50</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>50</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1">
-        <v>50</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>50</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1">
-        <v>50</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1">
-        <v>50</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1">
-        <v>50</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="1">
-        <v>50</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="1">
-        <v>50</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1">
-        <v>50</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1">
-        <v>50</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1">
-        <v>50</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1">
-        <v>50</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="1">
-        <v>50</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="1">
-        <v>50</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="1">
-        <v>50</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="1">
-        <v>50</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="1">
-        <v>50</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="1">
-        <v>50</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="1">
-        <v>50</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="1">
-        <v>50</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="1">
-        <v>50</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="1">
-        <v>50</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="1">
-        <v>50</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="1">
-        <v>50</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="1">
-        <v>50</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="1">
-        <v>50</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="1">
-        <v>50</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="1">
-        <v>50</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="1">
-        <v>50</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" s="1">
-        <v>50</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="1">
-        <v>50</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="1">
-        <v>50</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="1">
-        <v>50</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="1">
-        <v>50</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="1">
-        <v>50</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="1">
-        <v>50</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="1">
-        <v>50</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="1">
-        <v>50</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D52" s="1">
-        <v>50</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D53" s="1">
-        <v>50</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="1">
-        <v>50</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="1">
-        <v>50</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56" s="1">
-        <v>50</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D57" s="1">
-        <v>50</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="1">
-        <v>50</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D59" s="1">
-        <v>50</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="1">
-        <v>50</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D61" s="1">
-        <v>50</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E62" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,8 +2519,8 @@
       <c r="D2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="10">
-        <v>5380</v>
+      <c r="E2" s="10" t="s">
+        <v>444</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>54</v>
@@ -3649,8 +2614,8 @@
       <c r="D3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="10">
-        <v>1150</v>
+      <c r="E3" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>54</v>
@@ -3667,8 +2632,8 @@
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="12">
-        <v>44179</v>
+      <c r="M3" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>68</v>
@@ -3746,8 +2711,8 @@
       <c r="D4" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="10">
-        <v>1150</v>
+      <c r="E4" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>54</v>
@@ -3764,8 +2729,8 @@
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="12">
-        <v>44179</v>
+      <c r="M4" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>76</v>
@@ -3843,8 +2808,8 @@
       <c r="D5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="10">
-        <v>1150</v>
+      <c r="E5" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>54</v>
@@ -3861,8 +2826,8 @@
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="12">
-        <v>44179</v>
+      <c r="M5" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>76</v>
@@ -3940,8 +2905,8 @@
       <c r="D6" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="10">
-        <v>1150</v>
+      <c r="E6" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>54</v>
@@ -3958,8 +2923,8 @@
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="10"/>
-      <c r="M6" s="12">
-        <v>44179</v>
+      <c r="M6" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>76</v>
@@ -4037,8 +3002,8 @@
       <c r="D7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="10">
-        <v>1150</v>
+      <c r="E7" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>54</v>
@@ -4055,8 +3020,8 @@
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="12">
-        <v>44179</v>
+      <c r="M7" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>76</v>
@@ -4134,8 +3099,8 @@
       <c r="D8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="10">
-        <v>1150</v>
+      <c r="E8" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>54</v>
@@ -4152,8 +3117,8 @@
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="12">
-        <v>44179</v>
+      <c r="M8" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>76</v>
@@ -4231,8 +3196,8 @@
       <c r="D9" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="10">
-        <v>1150</v>
+      <c r="E9" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>54</v>
@@ -4249,8 +3214,8 @@
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="12">
-        <v>44179</v>
+      <c r="M9" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>76</v>
@@ -4328,8 +3293,8 @@
       <c r="D10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="10">
-        <v>1150</v>
+      <c r="E10" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>54</v>
@@ -4346,8 +3311,8 @@
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="12">
-        <v>44179</v>
+      <c r="M10" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>76</v>
@@ -4425,8 +3390,8 @@
       <c r="D11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="10">
-        <v>1150</v>
+      <c r="E11" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>54</v>
@@ -4443,8 +3408,8 @@
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="12">
-        <v>44179</v>
+      <c r="M11" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>76</v>
@@ -4522,8 +3487,8 @@
       <c r="D12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="10">
-        <v>2123</v>
+      <c r="E12" s="10" t="s">
+        <v>446</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>54</v>
@@ -4617,8 +3582,8 @@
       <c r="D13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="10">
-        <v>2036</v>
+      <c r="E13" s="10" t="s">
+        <v>447</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>54</v>
@@ -4712,8 +3677,8 @@
       <c r="D14" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="10">
-        <v>2036</v>
+      <c r="E14" s="10" t="s">
+        <v>447</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>54</v>
@@ -4807,8 +3772,8 @@
       <c r="D15" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="10">
-        <v>2036</v>
+      <c r="E15" s="10" t="s">
+        <v>447</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>54</v>
@@ -4902,8 +3867,8 @@
       <c r="D16" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="10">
-        <v>1044</v>
+      <c r="E16" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>54</v>
@@ -4997,8 +3962,8 @@
       <c r="D17" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="10">
-        <v>1044</v>
+      <c r="E17" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>54</v>
@@ -5092,8 +4057,8 @@
       <c r="D18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="10">
-        <v>1044</v>
+      <c r="E18" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>54</v>
@@ -5187,8 +4152,8 @@
       <c r="D19" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="10">
-        <v>1044</v>
+      <c r="E19" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>54</v>
@@ -5282,8 +4247,8 @@
       <c r="D20" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="10">
-        <v>1044</v>
+      <c r="E20" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>54</v>
@@ -5377,8 +4342,8 @@
       <c r="D21" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="10">
-        <v>1044</v>
+      <c r="E21" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>54</v>
@@ -5472,8 +4437,8 @@
       <c r="D22" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="10">
-        <v>1044</v>
+      <c r="E22" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>54</v>
@@ -5567,8 +4532,8 @@
       <c r="D23" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E23" s="10">
-        <v>1044</v>
+      <c r="E23" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>54</v>
@@ -5662,8 +4627,8 @@
       <c r="D24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="10">
-        <v>1044</v>
+      <c r="E24" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>54</v>
@@ -5757,8 +4722,8 @@
       <c r="D25" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="10">
-        <v>1044</v>
+      <c r="E25" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>54</v>
@@ -5852,8 +4817,8 @@
       <c r="D26" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="10">
-        <v>1044</v>
+      <c r="E26" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>54</v>
@@ -5947,8 +4912,8 @@
       <c r="D27" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="10">
-        <v>1044</v>
+      <c r="E27" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>54</v>
@@ -6042,8 +5007,8 @@
       <c r="D28" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="10">
-        <v>1044</v>
+      <c r="E28" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>54</v>
@@ -6137,8 +5102,8 @@
       <c r="D29" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="10">
-        <v>1044</v>
+      <c r="E29" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>54</v>
@@ -6232,8 +5197,8 @@
       <c r="D30" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="10">
-        <v>1044</v>
+      <c r="E30" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>54</v>
@@ -6327,8 +5292,8 @@
       <c r="D31" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="10">
-        <v>1044</v>
+      <c r="E31" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>54</v>
@@ -6422,8 +5387,8 @@
       <c r="D32" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="10">
-        <v>1044</v>
+      <c r="E32" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>54</v>
@@ -6517,8 +5482,8 @@
       <c r="D33" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="10">
-        <v>1044</v>
+      <c r="E33" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>54</v>
@@ -6612,8 +5577,8 @@
       <c r="D34" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E34" s="10">
-        <v>1044</v>
+      <c r="E34" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>54</v>
@@ -6707,8 +5672,8 @@
       <c r="D35" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E35" s="10">
-        <v>1044</v>
+      <c r="E35" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>54</v>
@@ -6802,8 +5767,8 @@
       <c r="D36" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="10">
-        <v>1044</v>
+      <c r="E36" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>54</v>
@@ -6897,8 +5862,8 @@
       <c r="D37" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="10">
-        <v>1044</v>
+      <c r="E37" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>54</v>
@@ -6992,8 +5957,8 @@
       <c r="D38" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="10">
-        <v>1044</v>
+      <c r="E38" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>54</v>
@@ -7087,8 +6052,8 @@
       <c r="D39" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E39" s="10">
-        <v>1044</v>
+      <c r="E39" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>54</v>
@@ -7182,8 +6147,8 @@
       <c r="D40" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E40" s="10">
-        <v>1044</v>
+      <c r="E40" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>54</v>
@@ -7277,8 +6242,8 @@
       <c r="D41" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E41" s="10">
-        <v>1044</v>
+      <c r="E41" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>54</v>
@@ -7372,8 +6337,8 @@
       <c r="D42" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E42" s="10">
-        <v>1044</v>
+      <c r="E42" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>54</v>
@@ -7467,8 +6432,8 @@
       <c r="D43" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E43" s="10">
-        <v>5002</v>
+      <c r="E43" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>54</v>
@@ -7562,8 +6527,8 @@
       <c r="D44" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E44" s="10">
-        <v>5002</v>
+      <c r="E44" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>54</v>
@@ -7657,8 +6622,8 @@
       <c r="D45" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E45" s="10">
-        <v>5002</v>
+      <c r="E45" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>54</v>
@@ -7752,8 +6717,8 @@
       <c r="D46" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="10">
-        <v>5002</v>
+      <c r="E46" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>54</v>
@@ -7847,8 +6812,8 @@
       <c r="D47" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E47" s="10">
-        <v>5002</v>
+      <c r="E47" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>54</v>
@@ -7942,8 +6907,8 @@
       <c r="D48" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E48" s="10">
-        <v>5002</v>
+      <c r="E48" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>54</v>
@@ -8037,8 +7002,8 @@
       <c r="D49" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E49" s="10">
-        <v>5002</v>
+      <c r="E49" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>54</v>
@@ -8132,8 +7097,8 @@
       <c r="D50" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E50" s="10">
-        <v>5002</v>
+      <c r="E50" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>54</v>
@@ -8227,8 +7192,8 @@
       <c r="D51" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E51" s="10">
-        <v>5002</v>
+      <c r="E51" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>54</v>
@@ -8322,8 +7287,8 @@
       <c r="D52" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E52" s="10">
-        <v>5002</v>
+      <c r="E52" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>54</v>
@@ -8417,8 +7382,8 @@
       <c r="D53" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E53" s="10">
-        <v>5002</v>
+      <c r="E53" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>54</v>
@@ -8512,8 +7477,8 @@
       <c r="D54" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E54" s="10">
-        <v>5002</v>
+      <c r="E54" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>54</v>
@@ -8607,8 +7572,8 @@
       <c r="D55" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E55" s="10">
-        <v>5002</v>
+      <c r="E55" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>54</v>
@@ -8702,8 +7667,8 @@
       <c r="D56" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="10">
-        <v>5002</v>
+      <c r="E56" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>54</v>
@@ -8797,8 +7762,8 @@
       <c r="D57" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E57" s="10">
-        <v>5002</v>
+      <c r="E57" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>54</v>
@@ -8892,8 +7857,8 @@
       <c r="D58" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E58" s="10">
-        <v>5002</v>
+      <c r="E58" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>54</v>
@@ -8987,8 +7952,8 @@
       <c r="D59" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E59" s="10">
-        <v>5002</v>
+      <c r="E59" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>54</v>
@@ -9082,8 +8047,8 @@
       <c r="D60" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E60" s="10">
-        <v>5002</v>
+      <c r="E60" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>54</v>
@@ -9177,8 +8142,8 @@
       <c r="D61" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E61" s="10">
-        <v>5002</v>
+      <c r="E61" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>54</v>
@@ -9272,8 +8237,8 @@
       <c r="D62" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E62" s="10">
-        <v>5002</v>
+      <c r="E62" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>54</v>
@@ -9367,8 +8332,8 @@
       <c r="D63" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E63" s="10">
-        <v>5002</v>
+      <c r="E63" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>54</v>
@@ -9462,8 +8427,8 @@
       <c r="D64" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E64" s="10">
-        <v>5002</v>
+      <c r="E64" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>54</v>
@@ -9557,8 +8522,8 @@
       <c r="D65" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E65" s="10">
-        <v>5002</v>
+      <c r="E65" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>54</v>
@@ -9652,8 +8617,8 @@
       <c r="D66" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E66" s="10">
-        <v>5002</v>
+      <c r="E66" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>54</v>
@@ -9747,8 +8712,8 @@
       <c r="D67" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E67" s="10">
-        <v>5002</v>
+      <c r="E67" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>54</v>
@@ -9842,8 +8807,8 @@
       <c r="D68" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E68" s="10">
-        <v>5002</v>
+      <c r="E68" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>54</v>
@@ -9937,8 +8902,8 @@
       <c r="D69" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E69" s="10">
-        <v>5002</v>
+      <c r="E69" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>54</v>
@@ -10032,8 +8997,8 @@
       <c r="D70" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E70" s="10">
-        <v>5002</v>
+      <c r="E70" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>54</v>
@@ -10127,8 +9092,8 @@
       <c r="D71" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E71" s="10">
-        <v>5002</v>
+      <c r="E71" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>54</v>
@@ -10222,8 +9187,8 @@
       <c r="D72" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E72" s="10">
-        <v>5002</v>
+      <c r="E72" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>54</v>
@@ -10317,8 +9282,8 @@
       <c r="D73" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E73" s="10">
-        <v>5002</v>
+      <c r="E73" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>54</v>
@@ -10412,8 +9377,8 @@
       <c r="D74" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E74" s="10">
-        <v>5002</v>
+      <c r="E74" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>54</v>
@@ -10507,8 +9472,8 @@
       <c r="D75" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E75" s="10">
-        <v>5002</v>
+      <c r="E75" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>54</v>
@@ -10602,8 +9567,8 @@
       <c r="D76" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E76" s="10">
-        <v>5002</v>
+      <c r="E76" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>54</v>
@@ -10697,8 +9662,8 @@
       <c r="D77" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E77" s="10">
-        <v>5002</v>
+      <c r="E77" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>54</v>
@@ -10792,8 +9757,8 @@
       <c r="D78" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E78" s="10">
-        <v>5002</v>
+      <c r="E78" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>54</v>
@@ -10887,8 +9852,8 @@
       <c r="D79" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E79" s="10">
-        <v>5002</v>
+      <c r="E79" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>54</v>
@@ -10982,8 +9947,8 @@
       <c r="D80" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="10">
-        <v>5002</v>
+      <c r="E80" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>54</v>
@@ -11077,8 +10042,8 @@
       <c r="D81" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E81" s="10">
-        <v>5002</v>
+      <c r="E81" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>54</v>
@@ -11172,8 +10137,8 @@
       <c r="D82" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E82" s="10">
-        <v>5002</v>
+      <c r="E82" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>54</v>
@@ -11267,8 +10232,8 @@
       <c r="D83" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E83" s="10">
-        <v>5002</v>
+      <c r="E83" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>54</v>
@@ -11362,8 +10327,8 @@
       <c r="D84" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E84" s="10">
-        <v>5002</v>
+      <c r="E84" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>54</v>
@@ -11457,8 +10422,8 @@
       <c r="D85" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E85" s="10">
-        <v>5002</v>
+      <c r="E85" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>54</v>
@@ -11552,8 +10517,8 @@
       <c r="D86" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E86" s="10">
-        <v>5002</v>
+      <c r="E86" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>54</v>
@@ -11647,8 +10612,8 @@
       <c r="D87" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E87" s="10">
-        <v>5002</v>
+      <c r="E87" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>54</v>
@@ -11742,8 +10707,8 @@
       <c r="D88" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E88" s="10">
-        <v>5002</v>
+      <c r="E88" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>54</v>
@@ -11837,8 +10802,8 @@
       <c r="D89" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E89" s="10">
-        <v>5002</v>
+      <c r="E89" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>54</v>
@@ -11932,8 +10897,8 @@
       <c r="D90" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E90" s="10">
-        <v>5002</v>
+      <c r="E90" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>54</v>
@@ -12027,8 +10992,8 @@
       <c r="D91" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E91" s="10">
-        <v>5002</v>
+      <c r="E91" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>54</v>
@@ -12122,8 +11087,8 @@
       <c r="D92" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E92" s="10">
-        <v>5002</v>
+      <c r="E92" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>54</v>
@@ -12217,8 +11182,8 @@
       <c r="D93" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E93" s="10">
-        <v>5002</v>
+      <c r="E93" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>54</v>
@@ -12312,8 +11277,8 @@
       <c r="D94" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E94" s="10">
-        <v>5002</v>
+      <c r="E94" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>54</v>
@@ -12407,8 +11372,8 @@
       <c r="D95" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E95" s="10">
-        <v>5002</v>
+      <c r="E95" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>54</v>
@@ -12502,8 +11467,8 @@
       <c r="D96" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E96" s="10">
-        <v>5002</v>
+      <c r="E96" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>54</v>
@@ -12597,8 +11562,8 @@
       <c r="D97" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E97" s="10">
-        <v>5002</v>
+      <c r="E97" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>54</v>
@@ -12692,8 +11657,8 @@
       <c r="D98" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E98" s="10">
-        <v>5002</v>
+      <c r="E98" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>54</v>
@@ -12787,8 +11752,8 @@
       <c r="D99" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E99" s="10">
-        <v>5002</v>
+      <c r="E99" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>54</v>
@@ -12882,8 +11847,8 @@
       <c r="D100" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E100" s="10">
-        <v>5002</v>
+      <c r="E100" s="10" t="s">
+        <v>448</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>54</v>
@@ -12968,4 +11933,1068 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D8" s="1">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="1">
+        <v>700</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D10" s="1">
+        <v>700</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>50</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1">
+        <v>50</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1">
+        <v>50</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1">
+        <v>50</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <v>50</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1">
+        <v>50</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="1">
+        <v>50</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1">
+        <v>50</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1">
+        <v>50</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1">
+        <v>50</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <v>50</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="1">
+        <v>50</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1">
+        <v>50</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="1">
+        <v>50</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="1">
+        <v>50</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="1">
+        <v>50</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1">
+        <v>50</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1">
+        <v>50</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="1">
+        <v>50</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="1">
+        <v>50</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="1">
+        <v>50</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="1">
+        <v>50</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="1">
+        <v>50</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="1">
+        <v>50</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="1">
+        <v>50</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="1">
+        <v>50</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="1">
+        <v>50</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="1">
+        <v>50</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="1">
+        <v>50</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="1">
+        <v>50</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="1">
+        <v>50</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="1">
+        <v>50</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="1">
+        <v>50</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="1">
+        <v>50</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="1">
+        <v>50</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="1">
+        <v>50</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="1">
+        <v>50</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="1">
+        <v>50</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="1">
+        <v>50</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="1">
+        <v>50</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1">
+        <v>50</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E62" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>